<commit_message>
running sims on the new ac3 cluster
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81CFD81-C379-4799-96F8-41EB284B82E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F48AE18-C8BF-4D9F-AF32-946BE19B2357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>With burnin (scale = 0.033, ml = c(5, 50, 250), ml_expt = 2)</t>
+  </si>
+  <si>
+    <t>Set_14</t>
+  </si>
+  <si>
+    <t>With burnin (scale = 0.033, ml = 0.5, ml_expt = 2, mut_ratio = 0.02)</t>
   </si>
 </sst>
 </file>
@@ -553,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F767BA-E529-4BB9-8A9B-635D3AE84CE5}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1037,7 +1043,7 @@
         <v>300</v>
       </c>
       <c r="D14" s="2">
-        <v>45311</v>
+        <v>45677</v>
       </c>
       <c r="E14">
         <v>284315</v>
@@ -1063,7 +1069,7 @@
         <v>200</v>
       </c>
       <c r="D15" s="2">
-        <v>45335</v>
+        <v>45701</v>
       </c>
       <c r="K15" t="s">
         <v>30</v>
@@ -1080,10 +1086,24 @@
         <v>300</v>
       </c>
       <c r="D16" s="2">
-        <v>45348</v>
+        <v>45714</v>
       </c>
       <c r="E16">
         <v>284591</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17">
+        <v>100</v>
+      </c>
+      <c r="D17" s="2">
+        <v>45734</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
params and new data
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3CF3BA2-09BE-409C-B5CF-3A5E0F813BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40445410-D1F9-43FF-A9B5-0A93784E2238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7360" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="53">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>job_261756 (ac3)</t>
+  </si>
+  <si>
+    <t>262033 (ac3)</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -242,12 +248,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F767BA-E529-4BB9-8A9B-635D3AE84CE5}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1094,8 +1101,11 @@
       <c r="E16">
         <v>284591</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="J16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1110,6 +1120,21 @@
       </c>
       <c r="E17" t="s">
         <v>50</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="5">
+        <v>45736</v>
+      </c>
+      <c r="I17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Recalculating true V_A and lost_Va
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E1B32C-6AD6-4F96-8D01-61952C69D279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25D45EF-ABF1-4C5C-8EBD-F4A83DB93BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
+    <sheet name="Rcalculate true V_A &amp; V_a_left" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="70">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -225,7 +226,25 @@
     <t>09-Jan-25, 18-Mar-2025</t>
   </si>
   <si>
-    <t>job_262387 (ac3)</t>
+    <t>job_262387 (ac3) for 1-65; 284708 (qm) for 66-100 [the ac3 job array stopped because of maintenance on ac3]</t>
+  </si>
+  <si>
+    <t>Set(s)</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Job ID</t>
+  </si>
+  <si>
+    <t>Set_9, Set_15a, Set_15_b</t>
+  </si>
+  <si>
+    <t>Standard set for sims with burnin and sims with larger scales</t>
   </si>
 </sst>
 </file>
@@ -603,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F767BA-E529-4BB9-8A9B-635D3AE84CE5}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1338,4 +1357,59 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E757BB-1C2C-4D1E-BA64-CFB54311D593}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" customWidth="1"/>
+    <col min="4" max="4" width="16.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2">
+        <v>300</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45723</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Latex code backups and new figures
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D43E404-3EFA-4F3A-AA28-12EAA78EE1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFE729A-9AE5-4CB8-8373-94AAFD6A8270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="75">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>With burnin, mut_ratio = c(0.0002, 0.02)</t>
+  </si>
+  <si>
+    <t>267768 (new_ac3)</t>
   </si>
 </sst>
 </file>
@@ -1398,7 +1401,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1406,6 +1409,7 @@
     <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.26953125" customWidth="1"/>
     <col min="4" max="4" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -1458,6 +1462,9 @@
       <c r="D3" s="2">
         <v>45755</v>
       </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
params and script to make plots
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C4E276-91DA-4C9A-9BB0-3734FA824258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA27AAEB-8699-4B09-9934-AB308CEA4B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="75">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>Set_12</t>
+  </si>
+  <si>
+    <t>283727 (new_ac3)</t>
   </si>
 </sst>
 </file>
@@ -1384,7 +1387,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1469,6 +1472,9 @@
       <c r="D4" s="2">
         <v>45757</v>
       </c>
+      <c r="E4" s="2">
+        <v>45759</v>
+      </c>
       <c r="F4">
         <v>284735</v>
       </c>
@@ -1485,6 +1491,9 @@
       </c>
       <c r="D5" s="2">
         <v>45757</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
running on eddie test
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B96743-7490-4E60-A506-D006C085866F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865ECB2A-3F5A-4FB8-B1B6-E8E3CF595D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="98">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -327,6 +327,9 @@
   </si>
   <si>
     <t>Set_17</t>
+  </si>
+  <si>
+    <t>319110 (new_ac3)</t>
   </si>
 </sst>
 </file>
@@ -724,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F767BA-E529-4BB9-8A9B-635D3AE84CE5}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1507,6 +1510,9 @@
       </c>
       <c r="H23" s="2">
         <v>45781</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
separate parameter grid to run analyses on qmaster
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865ECB2A-3F5A-4FB8-B1B6-E8E3CF595D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C9C6E8-6FE2-4DE5-837C-A98E1B5ADB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="101">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -330,6 +330,15 @@
   </si>
   <si>
     <t>319110 (new_ac3)</t>
+  </si>
+  <si>
+    <t>Corrected_analysis_start_date</t>
+  </si>
+  <si>
+    <t>Corrected_analysis_job_ID</t>
+  </si>
+  <si>
+    <t>332960 (new_ac3)</t>
   </si>
 </sst>
 </file>
@@ -725,16 +734,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F767BA-E529-4BB9-8A9B-635D3AE84CE5}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="130.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.26953125" customWidth="1"/>
     <col min="4" max="4" width="20.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.6328125" bestFit="1" customWidth="1"/>
@@ -744,9 +753,12 @@
     <col min="9" max="9" width="19.08984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -780,8 +792,20 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -816,7 +840,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -851,7 +875,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -886,7 +910,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -921,7 +945,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -956,7 +980,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -991,7 +1015,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1026,7 +1050,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1061,7 +1085,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1096,7 +1120,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>35</v>
       </c>
@@ -1130,8 +1154,14 @@
       <c r="K11" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L11" s="4">
+        <v>45790</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1166,7 +1196,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
@@ -1201,7 +1231,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
@@ -1236,7 +1266,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
@@ -1271,7 +1301,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>46</v>
       </c>
@@ -1303,7 +1333,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>48</v>
       </c>
@@ -1335,7 +1365,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>53</v>
       </c>
@@ -1367,7 +1397,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>53</v>
       </c>
@@ -1399,7 +1429,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>57</v>
       </c>
@@ -1428,7 +1458,7 @@
         <v>284663</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>58</v>
       </c>
@@ -1457,7 +1487,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>88</v>
       </c>
@@ -1485,8 +1515,17 @@
       <c r="I22" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" s="2">
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>96</v>
       </c>
@@ -1513,6 +1552,12 @@
       </c>
       <c r="I23" s="3" t="s">
         <v>97</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1527,7 +1572,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
changed output path on Eddie
Earlier it was set inside the scratch directory where files older than a month are deleted
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C9A218-2E44-4852-B4F2-2BB6984DECF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E225C188-7725-4B98-934C-0C158727C16B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="102">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>332960 (new_ac3)</t>
+  </si>
+  <si>
+    <t>48690588 (Eddie)</t>
   </si>
 </sst>
 </file>
@@ -736,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F767BA-E529-4BB9-8A9B-635D3AE84CE5}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1014,6 +1017,18 @@
       <c r="K7" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="L7" s="4">
+        <v>45791</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="N7" s="4">
+        <v>45791</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -1229,6 +1244,9 @@
       </c>
       <c r="K13" s="3" t="s">
         <v>34</v>
+      </c>
+      <c r="L13" s="4">
+        <v>45792</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Set_9 (all.gp = TRUE) params
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7199B527-BC2D-4F36-A4E3-9172814B7CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B55D7D-525C-40E3-B6D9-033A961FC144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="114">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -411,6 +411,9 @@
   </si>
   <si>
     <t>346640 (new_ac3)</t>
+  </si>
+  <si>
+    <t>48782249 (Eddie)</t>
   </si>
 </sst>
 </file>
@@ -973,8 +976,8 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N22" sqref="N22"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1564,10 +1567,18 @@
       <c r="K14" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="23"/>
+      <c r="L14" s="22">
+        <v>45800</v>
+      </c>
+      <c r="M14" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="N14" s="22">
+        <v>45802</v>
+      </c>
+      <c r="O14" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="20" t="s">
@@ -1657,7 +1668,9 @@
       <c r="N16" s="22">
         <v>45797</v>
       </c>
-      <c r="O16" s="23"/>
+      <c r="O16" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="17" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
@@ -1700,7 +1713,9 @@
       <c r="N17" s="22">
         <v>45798</v>
       </c>
-      <c r="O17" s="23"/>
+      <c r="O17" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="18" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">

</xml_diff>

<commit_message>
Set_9 fixed NE params
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3A9AA7-CE9C-492E-AE93-40F69FBDA3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E8F7C2-62F0-494E-970E-6120B482C6E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="116">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t>48813679 (Eddie)</t>
+  </si>
+  <si>
+    <t>48828582 (Eddie)</t>
   </si>
 </sst>
 </file>
@@ -617,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -661,6 +664,12 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -980,7 +989,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L19" sqref="L19"/>
+      <selection pane="topRight" activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1798,7 +1807,9 @@
       <c r="L19" s="22">
         <v>45804</v>
       </c>
-      <c r="M19" s="21"/>
+      <c r="M19" s="21" t="s">
+        <v>115</v>
+      </c>
       <c r="N19" s="21"/>
       <c r="O19" s="23"/>
     </row>
@@ -1835,7 +1846,7 @@
       <c r="L20" s="31">
         <v>45798</v>
       </c>
-      <c r="M20" s="30" t="s">
+      <c r="M20" s="32" t="s">
         <v>107</v>
       </c>
       <c r="N20" s="31">
@@ -1874,7 +1885,7 @@
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
       <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
+      <c r="M21" s="32"/>
       <c r="N21" s="30"/>
       <c r="O21" s="23"/>
     </row>
@@ -1915,7 +1926,7 @@
       <c r="L22" s="22">
         <v>45791</v>
       </c>
-      <c r="M22" s="21">
+      <c r="M22" s="33">
         <v>284912</v>
       </c>
       <c r="N22" s="22">

</xml_diff>

<commit_message>
params for Set_18_std pool_seq analyses
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E8F7C2-62F0-494E-970E-6120B482C6E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00046CF0-8B62-464E-A445-85E778A1E021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
-    <sheet name="Rcalculate true V_A &amp; V_a_left" sheetId="2" r:id="rId2"/>
-    <sheet name="Recalculate BC_V_A" sheetId="3" r:id="rId3"/>
+    <sheet name="Pool_seq_analyses" sheetId="4" r:id="rId2"/>
+    <sheet name="Rcalculate true V_A &amp; V_a_left" sheetId="2" r:id="rId3"/>
+    <sheet name="Recalculate BC_V_A" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="118">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -420,6 +421,12 @@
   </si>
   <si>
     <t>48828582 (Eddie)</t>
+  </si>
+  <si>
+    <t>Set_18_std</t>
+  </si>
+  <si>
+    <t>Standard set without burnin analysed with simulations pf poolseq (read_length = 75, coverage = 1000, V_logmean = 0)</t>
   </si>
 </sst>
 </file>
@@ -660,16 +667,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -987,9 +994,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F767BA-E529-4BB9-8A9B-635D3AE84CE5}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M22" sqref="M22"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1846,7 +1853,7 @@
       <c r="L20" s="31">
         <v>45798</v>
       </c>
-      <c r="M20" s="32" t="s">
+      <c r="M20" s="33" t="s">
         <v>107</v>
       </c>
       <c r="N20" s="31">
@@ -1884,9 +1891,9 @@
       </c>
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="30"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="32"/>
       <c r="O21" s="23"/>
     </row>
     <row r="22" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1926,7 +1933,7 @@
       <c r="L22" s="22">
         <v>45791</v>
       </c>
-      <c r="M22" s="33">
+      <c r="M22" s="30">
         <v>284912</v>
       </c>
       <c r="N22" s="22">
@@ -2036,6 +2043,66 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B83F06-536D-4FC4-A19B-2685788EFCD2}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45829</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E757BB-1C2C-4D1E-BA64-CFB54311D593}">
   <dimension ref="A1:G12"/>
   <sheetViews>
@@ -2297,7 +2364,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8D10C7-D493-4278-B869-F549E3A19DCB}">
   <dimension ref="A1:F2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Pool_seq full sims params
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B3A8E7-EB99-4F3C-9BF1-8FCB66695085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFC6AAF-58C8-48F0-8EE0-1A99A92C2277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="128">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -448,6 +448,15 @@
   </si>
   <si>
     <t>Standard set without burnin analysed with simulations pf poolseq (read_length = 1, coverage = 1000, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Eddie 49330882</t>
+  </si>
+  <si>
+    <t>Set_9_std</t>
+  </si>
+  <si>
+    <t>Standard set with burnin analysed with simulations pf poolseq (read_length = 75, coverage = 1000, V_logmean = 0)</t>
   </si>
 </sst>
 </file>
@@ -2065,10 +2074,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B83F06-536D-4FC4-A19B-2685788EFCD2}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F5" sqref="F5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2184,6 +2193,29 @@
         <v>100</v>
       </c>
       <c r="D5" s="2">
+        <v>45830</v>
+      </c>
+      <c r="E5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45830</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6" s="2">
         <v>45830</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified fit.model() to accommodate simulate_pool_seq()
Applying simulate_pool_seq() sometimes results in some sites not being covered at all which then get assigned NAs for allele frequency. This would mean that every element of the projected allele frequency change becomes NA resulting in the asreml model failing.

To account for this, modified fit.model() such that wherever pbar1 or pbar2 have an NA, those elements in both pbar1 and pbar2 get turned into 0s.
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB812F9A-7E6C-4C8A-A610-A29AC95231D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA6AB3D-0175-4584-9E7F-13BF01126990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -459,7 +459,7 @@
     <t>Standard set with burnin analysed with simulations pf poolseq (read_length = 75, coverage = 1000, V_logmean = 0)</t>
   </si>
   <si>
-    <t>Eddie 49331096</t>
+    <t>Eddie 49372742</t>
   </si>
 </sst>
 </file>
@@ -2080,7 +2080,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2219,7 +2219,7 @@
         <v>100</v>
       </c>
       <c r="D6" s="2">
-        <v>45830</v>
+        <v>45834</v>
       </c>
       <c r="E6" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
test dominance sim params
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE48819B-3739-47B4-9075-77D0388CB9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703888AB-9B5F-4707-8A75-950405BFAC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="137">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -481,6 +481,9 @@
   </si>
   <si>
     <t>1 task did not complete</t>
+  </si>
+  <si>
+    <t>Eddie 49404027</t>
   </si>
 </sst>
 </file>
@@ -2101,7 +2104,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2268,6 +2271,9 @@
       <c r="E7" t="s">
         <v>131</v>
       </c>
+      <c r="F7" s="2">
+        <v>45842</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -2304,6 +2310,9 @@
       </c>
       <c r="D9" s="2">
         <v>45841</v>
+      </c>
+      <c r="E9" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lost_va_script - fixed paths for Eddie
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C10D58-DAE5-4821-9119-D21DC9E72A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77655C37-2AB1-4DA7-A0A3-078054D5EF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="688" activeTab="2" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="163">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -559,6 +559,9 @@
   </si>
   <si>
     <t>49971494 (Eddie)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 49971535 (Eddie)</t>
   </si>
 </sst>
 </file>
@@ -1157,11 +1160,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F767BA-E529-4BB9-8A9B-635D3AE84CE5}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2333,7 +2336,30 @@
       <c r="G28" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="L28" s="35"/>
+      <c r="H28" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="K28" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="L28" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="M28" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="N28" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="O28" s="35" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="28" t="s">
@@ -2351,6 +2377,32 @@
       <c r="E29" s="31" t="s">
         <v>159</v>
       </c>
+      <c r="F29" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="K29" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="L29" s="39">
+        <v>45854</v>
+      </c>
+      <c r="M29" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="N29" s="41"/>
+      <c r="O29" s="41"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="28" t="s">
@@ -2368,6 +2420,28 @@
       <c r="E30" t="s">
         <v>160</v>
       </c>
+      <c r="F30" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="K30" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="L30" s="40"/>
+      <c r="M30" s="41"/>
+      <c r="N30" s="41"/>
+      <c r="O30" s="41"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="28" t="s">
@@ -2385,9 +2459,35 @@
       <c r="E31" s="31" t="s">
         <v>161</v>
       </c>
+      <c r="F31" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="K31" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="L31" s="40"/>
+      <c r="M31" s="41"/>
+      <c r="N31" s="41"/>
+      <c r="O31" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="L29:L31"/>
+    <mergeCell ref="M29:M31"/>
+    <mergeCell ref="N29:N31"/>
+    <mergeCell ref="O29:O31"/>
     <mergeCell ref="N20:N21"/>
     <mergeCell ref="L20:L21"/>
     <mergeCell ref="M20:M21"/>
@@ -2623,10 +2723,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E757BB-1C2C-4D1E-BA64-CFB54311D593}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2894,7 +2994,56 @@
         <v>145</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14" s="29">
+        <v>100</v>
+      </c>
+      <c r="D14" s="39">
+        <v>45854</v>
+      </c>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" s="29">
+        <v>100</v>
+      </c>
+      <c r="D15" s="39"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" s="29">
+        <v>100</v>
+      </c>
+      <c r="D16" s="39"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="F14:F16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
V_a in log files in history sim
Corrected the calculation of V_a in the log files generated by the History sim to account for dominance
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D303186F-3FEF-4B67-A5C1-2651FE47584A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24C80E5-6AEC-4DC8-8B5F-B043F27ED1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="688" activeTab="2" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="165">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -513,9 +513,6 @@
     <t>386160 (new_ac3)</t>
   </si>
   <si>
-    <t>Set_22a</t>
-  </si>
-  <si>
     <t>Full simulations with dominance (k = 0.5)</t>
   </si>
   <si>
@@ -565,6 +562,12 @@
   </si>
   <si>
     <t xml:space="preserve"> 49971591 (Eddie)</t>
+  </si>
+  <si>
+    <t>Set_24_A</t>
+  </si>
+  <si>
+    <t>49991210 (Eddie)</t>
   </si>
 </sst>
 </file>
@@ -829,6 +832,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -837,15 +849,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1161,13 +1164,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F767BA-E529-4BB9-8A9B-635D3AE84CE5}">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A29" sqref="A29:D31"/>
+      <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2021,13 +2024,13 @@
       </c>
       <c r="J20" s="21"/>
       <c r="K20" s="21"/>
-      <c r="L20" s="36">
+      <c r="L20" s="39">
         <v>45798</v>
       </c>
-      <c r="M20" s="38" t="s">
+      <c r="M20" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="N20" s="36">
+      <c r="N20" s="39">
         <v>45800</v>
       </c>
       <c r="O20" s="23"/>
@@ -2062,9 +2065,9 @@
       </c>
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="37"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="40"/>
       <c r="O21" s="23"/>
     </row>
     <row r="22" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2221,7 +2224,7 @@
         <v>13</v>
       </c>
       <c r="G25" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H25" s="29" t="s">
         <v>14</v>
@@ -2235,10 +2238,10 @@
       <c r="K25" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L25" s="39">
+      <c r="L25" s="36">
         <v>45843</v>
       </c>
-      <c r="M25" s="41" t="s">
+      <c r="M25" s="38" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2262,7 +2265,7 @@
         <v>13</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H26" s="29" t="s">
         <v>14</v>
@@ -2276,15 +2279,15 @@
       <c r="K26" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L26" s="40"/>
-      <c r="M26" s="41"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="38"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" s="29" t="s">
         <v>150</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>151</v>
       </c>
       <c r="C27" s="29">
         <v>100</v>
@@ -2293,13 +2296,13 @@
         <v>45845</v>
       </c>
       <c r="E27" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F27" s="31" t="s">
         <v>13</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H27" s="31" t="s">
         <v>14</v>
@@ -2317,27 +2320,18 @@
         <v>45845</v>
       </c>
       <c r="M27" s="32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A28" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="B28" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="C28" s="29">
-        <v>100</v>
-      </c>
       <c r="D28" s="2">
         <v>45843</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G28" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H28" s="29" t="s">
         <v>14</v>
@@ -2366,7 +2360,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B29" s="29" t="s">
         <v>143</v>
@@ -2378,7 +2372,7 @@
         <v>45854</v>
       </c>
       <c r="E29" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F29" s="29" t="s">
         <v>13</v>
@@ -2398,18 +2392,18 @@
       <c r="K29" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L29" s="39">
+      <c r="L29" s="36">
         <v>45854</v>
       </c>
-      <c r="M29" s="41" t="s">
-        <v>162</v>
-      </c>
-      <c r="N29" s="41"/>
-      <c r="O29" s="41"/>
+      <c r="M29" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="N29" s="38"/>
+      <c r="O29" s="38"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B30" s="29" t="s">
         <v>142</v>
@@ -2421,7 +2415,7 @@
         <v>45854</v>
       </c>
       <c r="E30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F30" s="29" t="s">
         <v>13</v>
@@ -2441,17 +2435,17 @@
       <c r="K30" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L30" s="40"/>
-      <c r="M30" s="41"/>
-      <c r="N30" s="41"/>
-      <c r="O30" s="41"/>
+      <c r="L30" s="37"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="38"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C31" s="29">
         <v>100</v>
@@ -2460,7 +2454,7 @@
         <v>45854</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F31" s="29" t="s">
         <v>13</v>
@@ -2480,10 +2474,27 @@
       <c r="K31" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L31" s="40"/>
-      <c r="M31" s="41"/>
-      <c r="N31" s="41"/>
-      <c r="O31" s="41"/>
+      <c r="L31" s="37"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="38"/>
+      <c r="O31" s="38"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A32" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="29">
+        <v>100</v>
+      </c>
+      <c r="D32" s="2">
+        <v>45855</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>164</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2673,7 +2684,7 @@
         <v>45844</v>
       </c>
       <c r="E7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F7" s="2">
         <v>45842</v>
@@ -2728,7 +2739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E757BB-1C2C-4D1E-BA64-CFB54311D593}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -2999,7 +3010,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B14" s="29" t="s">
         <v>143</v>
@@ -3007,17 +3018,17 @@
       <c r="C14" s="29">
         <v>100</v>
       </c>
-      <c r="D14" s="39">
+      <c r="D14" s="36">
         <v>45854</v>
       </c>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41" t="s">
-        <v>163</v>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B15" s="29" t="s">
         <v>142</v>
@@ -3025,23 +3036,23 @@
       <c r="C15" s="29">
         <v>100</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C16" s="29">
         <v>100</v>
       </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
scale=0.045 test with dominance
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24C80E5-6AEC-4DC8-8B5F-B043F27ED1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCCE7CB-494C-49A2-88FC-BE93F0124B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -567,7 +567,7 @@
     <t>Set_24_A</t>
   </si>
   <si>
-    <t>49991210 (Eddie)</t>
+    <t>49995815 (Eddie)</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1170,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Set_25_D params (for tasks that failed)
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB29DCD-9E4E-4F95-8D04-A83078EE0A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2BAD57-C1F2-46D0-BAE3-42923B500599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="171">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -577,6 +577,15 @@
   </si>
   <si>
     <t>50060065 (Eddie)</t>
+  </si>
+  <si>
+    <t>Set_25_D</t>
+  </si>
+  <si>
+    <t>Full simulations with dominance (k = 0.75)</t>
+  </si>
+  <si>
+    <t>50104052  (Eddie)</t>
   </si>
 </sst>
 </file>
@@ -1173,13 +1182,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F767BA-E529-4BB9-8A9B-635D3AE84CE5}">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2523,6 +2532,23 @@
       </c>
       <c r="F33" s="31" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="C34" s="29">
+        <v>100</v>
+      </c>
+      <c r="D34" s="2">
+        <v>45862</v>
+      </c>
+      <c r="E34" s="31" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set_26 poolseq coverage = 1000 params
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6C6EC5-12BE-4154-8D07-8892D62E35E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B61AE67-4EA0-450C-A234-B2EFC543FB3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="688" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" tabRatio="688" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="182">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -616,6 +616,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 50214717 (Eddie)</t>
+  </si>
+  <si>
+    <t>50215469 (Eddie)</t>
   </si>
 </sst>
 </file>
@@ -1216,11 +1219,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F767BA-E529-4BB9-8A9B-635D3AE84CE5}">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="G20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
+      <selection pane="bottomRight" activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2668,6 +2671,27 @@
       <c r="F35" s="36" t="s">
         <v>179</v>
       </c>
+      <c r="G35" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="K35" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="L35" s="2">
+        <v>45866</v>
+      </c>
+      <c r="M35" s="36" t="s">
+        <v>181</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2691,14 +2715,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B83F06-536D-4FC4-A19B-2685788EFCD2}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.90625" customWidth="1"/>
     <col min="4" max="4" width="18.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.1796875" bestFit="1" customWidth="1"/>
@@ -2907,9 +2931,8 @@
       <c r="A10" t="s">
         <v>177</v>
       </c>
-      <c r="B10" t="str">
-        <f>'Sims and main analysis'!$B$35</f>
-        <v>Simplified simulations varying the number of neutral sites</v>
+      <c r="B10" t="s">
+        <v>178</v>
       </c>
       <c r="C10">
         <v>100</v>

</xml_diff>

<commit_message>
Set_18 poolseq (coverage = 500) params
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8D182A-9AB7-4705-950F-24737F60FAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FABCDC3-6D42-43F0-BDE5-FB1B0D3D4F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" tabRatio="688" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="28635" yWindow="-165" windowWidth="29130" windowHeight="17610" tabRatio="688" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="186">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -622,6 +622,15 @@
   </si>
   <si>
     <t>Eddie 50217846</t>
+  </si>
+  <si>
+    <t>50221120 (Eddie)</t>
+  </si>
+  <si>
+    <t>Standard set without burnin analysed with simulations pf poolseq (read_length = 75, coverage = 500, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Standard set with burnin analysed with simulations pf poolseq (read_length = 75, coverage = 500, V_logmean = 0)</t>
   </si>
 </sst>
 </file>
@@ -2716,10 +2725,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B83F06-536D-4FC4-A19B-2685788EFCD2}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2849,45 +2858,40 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>184</v>
       </c>
       <c r="C6">
         <v>100</v>
       </c>
       <c r="D6" s="2">
-        <v>45835</v>
-      </c>
-      <c r="E6" t="s">
-        <v>135</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45836</v>
-      </c>
-      <c r="G6" t="s">
-        <v>129</v>
-      </c>
+        <v>45867</v>
+      </c>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>122</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C7">
         <v>100</v>
       </c>
       <c r="D7" s="2">
-        <v>45844</v>
+        <v>45835</v>
       </c>
       <c r="E7" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="F7" s="2">
-        <v>45842</v>
+        <v>45836</v>
+      </c>
+      <c r="G7" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -2895,22 +2899,19 @@
         <v>122</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C8">
         <v>100</v>
       </c>
       <c r="D8" s="2">
-        <v>45840</v>
+        <v>45844</v>
       </c>
       <c r="E8" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="F8" s="2">
-        <v>45841</v>
-      </c>
-      <c r="G8" t="s">
-        <v>133</v>
+        <v>45842</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -2918,32 +2919,67 @@
         <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C9">
         <v>100</v>
       </c>
       <c r="D9" s="2">
+        <v>45840</v>
+      </c>
+      <c r="E9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" s="2">
         <v>45841</v>
       </c>
-      <c r="E9" t="s">
-        <v>134</v>
+      <c r="G9" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10" s="2">
+        <v>45841</v>
+      </c>
+      <c r="E10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" t="s">
+        <v>185</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>177</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>178</v>
       </c>
-      <c r="C10">
-        <v>100</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C12">
+        <v>100</v>
+      </c>
+      <c r="D12" s="2">
         <v>45867</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E12" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2957,7 +2993,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3297,6 +3333,12 @@
       </c>
       <c r="C18" s="36">
         <v>100</v>
+      </c>
+      <c r="D18" s="2">
+        <v>45867</v>
+      </c>
+      <c r="F18" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set_9_std pool_seq analyses params
coverage = 500
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FABCDC3-6D42-43F0-BDE5-FB1B0D3D4F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CD9B73-4F75-4502-BE20-D4A1BBD50ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28635" yWindow="-165" windowWidth="29130" windowHeight="17610" tabRatio="688" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="187">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -631,6 +631,9 @@
   </si>
   <si>
     <t>Standard set with burnin analysed with simulations pf poolseq (read_length = 75, coverage = 500, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Eddie  50232357</t>
   </si>
 </sst>
 </file>
@@ -2728,7 +2731,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2868,6 +2871,9 @@
       </c>
       <c r="D6" s="2">
         <v>45867</v>
+      </c>
+      <c r="E6" t="s">
+        <v>186</v>
       </c>
       <c r="F6" s="2"/>
     </row>

</xml_diff>

<commit_message>
Set_25_D analysis params (LDalpha=TRUE)
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C4029B-1683-4996-BF08-1C7EA6F553BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7FCCBF-E705-4045-A730-A685A85EB5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28635" yWindow="-165" windowWidth="29130" windowHeight="17610" tabRatio="688" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="191">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -643,6 +643,9 @@
   </si>
   <si>
     <t>Without burnin standard set but with 65000 seg sites</t>
+  </si>
+  <si>
+    <t>50233753 (Eddie)</t>
   </si>
 </sst>
 </file>
@@ -1247,7 +1250,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
+      <selection pane="bottomRight" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2727,6 +2730,18 @@
       <c r="C36" s="36">
         <v>100</v>
       </c>
+      <c r="D36" s="2">
+        <v>45867</v>
+      </c>
+      <c r="E36" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="F36" s="2">
+        <v>45867</v>
+      </c>
+      <c r="G36" s="31" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2751,7 +2766,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Low ml_exp pool_seq params (100x)
Some modified figures as well
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925B8F9F-B975-44C4-B1E2-C50418D8E378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1058AA-5AA6-49BE-9AA2-899855317DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="688" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="688" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="202">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -667,6 +667,18 @@
   </si>
   <si>
     <t>50332951 (Eddie)</t>
+  </si>
+  <si>
+    <t>50351993 (Eddie)</t>
+  </si>
+  <si>
+    <t>Set_18 (r_exp = 0.01), Set_12</t>
+  </si>
+  <si>
+    <t>Simplified simulations varying the number of neutral sites (read_length = 75, coverage = 1000, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Simplified simulations with ml_exp = 0.01, and full simulations with ml_exp = 0.2 (read_length = 75, coverage = 100, V_logmean = 0)</t>
   </si>
 </sst>
 </file>
@@ -1267,11 +1279,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F767BA-E529-4BB9-8A9B-635D3AE84CE5}">
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M37" sqref="M37"/>
+      <selection pane="bottomRight" activeCell="G36" sqref="G36:K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2778,6 +2790,18 @@
       <c r="G36" s="31" t="s">
         <v>14</v>
       </c>
+      <c r="H36" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="K36" s="31" t="s">
+        <v>14</v>
+      </c>
       <c r="M36">
         <v>50307333</v>
       </c>
@@ -2840,10 +2864,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B83F06-536D-4FC4-A19B-2685788EFCD2}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3099,7 +3123,7 @@
         <v>177</v>
       </c>
       <c r="B12" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="C12">
         <v>100</v>
@@ -3109,6 +3133,20 @@
       </c>
       <c r="E12" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>199</v>
+      </c>
+      <c r="B13" t="s">
+        <v>201</v>
+      </c>
+      <c r="C13">
+        <v>200</v>
+      </c>
+      <c r="D13" s="2">
+        <v>45876</v>
       </c>
     </row>
   </sheetData>
@@ -3118,10 +3156,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E757BB-1C2C-4D1E-BA64-CFB54311D593}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3467,6 +3505,23 @@
       </c>
       <c r="F18" t="s">
         <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="C19" s="36">
+        <v>300</v>
+      </c>
+      <c r="D19" s="2">
+        <v>45876</v>
+      </c>
+      <c r="F19" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
poolseq analyses Set_12 and Set_18 params
100x
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1058AA-5AA6-49BE-9AA2-899855317DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFC847E-3093-4AEF-BC13-13471921D2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="688" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" tabRatio="688" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="205">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -672,13 +672,22 @@
     <t>50351993 (Eddie)</t>
   </si>
   <si>
-    <t>Set_18 (r_exp = 0.01), Set_12</t>
-  </si>
-  <si>
     <t>Simplified simulations varying the number of neutral sites (read_length = 75, coverage = 1000, V_logmean = 0)</t>
   </si>
   <si>
-    <t>Simplified simulations with ml_exp = 0.01, and full simulations with ml_exp = 0.2 (read_length = 75, coverage = 100, V_logmean = 0)</t>
+    <t>Eddie 50356330</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Set_12 (ml_exp = 0.2)</t>
+  </si>
+  <si>
+    <t>Set_18 (ml_exp = 0.01)</t>
+  </si>
+  <si>
+    <t>full simulations with ml_exp = 0.2 (read_length = 75, coverage = 100, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Simplified simulations with ml_exp = 0.01 (read_length = 75, coverage = 100, V_logmean = 0)</t>
   </si>
 </sst>
 </file>
@@ -2864,10 +2873,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B83F06-536D-4FC4-A19B-2685788EFCD2}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3123,7 +3132,7 @@
         <v>177</v>
       </c>
       <c r="B12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C12">
         <v>100</v>
@@ -3137,16 +3146,30 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B13" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C13">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D13" s="2">
         <v>45876</v>
+      </c>
+      <c r="E13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B14" t="s">
+        <v>203</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set_18 poolseq analysis params
500x
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFC847E-3093-4AEF-BC13-13471921D2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB5FE5C-3406-41F3-918E-F40710B5CA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" tabRatio="688" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="28635" yWindow="-165" windowWidth="29130" windowHeight="17610" tabRatio="688" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="207">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -675,9 +675,6 @@
     <t>Simplified simulations varying the number of neutral sites (read_length = 75, coverage = 1000, V_logmean = 0)</t>
   </si>
   <si>
-    <t>Eddie 50356330</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Set_12 (ml_exp = 0.2)</t>
   </si>
   <si>
@@ -688,6 +685,15 @@
   </si>
   <si>
     <t>Simplified simulations with ml_exp = 0.01 (read_length = 75, coverage = 100, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Eddie  50356395</t>
+  </si>
+  <si>
+    <t>ac3 422017</t>
+  </si>
+  <si>
+    <t>Simplified simulations with ml_exp = 0.01 (read_length = 75, coverage = 500, V_logmean = 0)</t>
   </si>
 </sst>
 </file>
@@ -2873,10 +2879,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B83F06-536D-4FC4-A19B-2685788EFCD2}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3146,30 +3152,50 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C13">
         <v>100</v>
       </c>
       <c r="D13" s="2">
-        <v>45876</v>
+        <v>45877</v>
       </c>
       <c r="E13" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>200</v>
+      </c>
+      <c r="B14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14" s="2">
+        <v>45877</v>
+      </c>
+      <c r="E14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>201</v>
       </c>
-      <c r="B14" t="s">
-        <v>203</v>
-      </c>
-      <c r="C14">
-        <v>100</v>
+      <c r="B15" t="s">
+        <v>206</v>
+      </c>
+      <c r="C15">
+        <v>100</v>
+      </c>
+      <c r="D15" s="2">
+        <v>45877</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set_29 corrected analysis params
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D9DB65-5E85-4BB8-AD47-CE63B06FEF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1E2972-A09F-4A13-B6AD-0F53B85D744C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="688" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" tabRatio="688" activeTab="2" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="225">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -737,6 +737,18 @@
   </si>
   <si>
     <t>Standard set with burnin (ml = 0.1)</t>
+  </si>
+  <si>
+    <t>50375206 (Eddie)</t>
+  </si>
+  <si>
+    <t>Standard set with burnin (ml = 0.1) (read_length = 75, coverage = 100, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Standard set with burnin (ml = 0.1) (read_length = 75, coverage = 500, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Standard set with burnin (ml = 0.1) (read_length = 75, coverage = 1000, V_logmean = 0)</t>
   </si>
 </sst>
 </file>
@@ -946,7 +958,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1025,6 +1037,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1341,11 +1354,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F767BA-E529-4BB9-8A9B-635D3AE84CE5}">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B38" sqref="B38"/>
+      <selection pane="bottomRight" activeCell="A38" sqref="A38:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2946,9 +2959,15 @@
       <c r="K38" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="L38" s="2"/>
-      <c r="M38" s="31"/>
-      <c r="N38" s="2"/>
+      <c r="L38" s="2">
+        <v>45880</v>
+      </c>
+      <c r="M38" s="31" t="s">
+        <v>221</v>
+      </c>
+      <c r="N38" s="2">
+        <v>45880</v>
+      </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="28" t="s">
@@ -3025,10 +3044,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B83F06-536D-4FC4-A19B-2685788EFCD2}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15:F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3393,6 +3412,39 @@
         <v>45877</v>
       </c>
     </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="48" t="s">
+        <v>217</v>
+      </c>
+      <c r="B18" s="48" t="s">
+        <v>222</v>
+      </c>
+      <c r="C18" s="48">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="48" t="s">
+        <v>217</v>
+      </c>
+      <c r="B19" s="48" t="s">
+        <v>223</v>
+      </c>
+      <c r="C19" s="48">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="48" t="s">
+        <v>217</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>224</v>
+      </c>
+      <c r="C20" s="48">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3400,10 +3452,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E757BB-1C2C-4D1E-BA64-CFB54311D593}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3782,18 +3834,32 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="C21" s="36">
+        <v>100</v>
+      </c>
+      <c r="D21" s="2">
+        <v>45880</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B22" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="C21" s="36">
+      <c r="C22" s="36">
         <v>300</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D22" s="2">
         <v>45876</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F22" t="s">
         <v>198</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Set_29 poolseq 100x params
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1E2972-A09F-4A13-B6AD-0F53B85D744C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F5DAF3-3339-4DC5-B49A-6220C0572CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" tabRatio="688" activeTab="2" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="226">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -749,6 +749,9 @@
   </si>
   <si>
     <t>Standard set with burnin (ml = 0.1) (read_length = 75, coverage = 1000, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>50382001 (Eddie)</t>
   </si>
 </sst>
 </file>
@@ -3455,7 +3458,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3844,6 +3847,9 @@
       </c>
       <c r="D21" s="2">
         <v>45880</v>
+      </c>
+      <c r="F21" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Set_29 poolseq (coverage = 500) params
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B96391-2D7F-4DFB-9507-BA88B1CB8662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E5C27C-8C3D-4EA9-A91E-EF968D06D634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28635" yWindow="-165" windowWidth="29130" windowHeight="17610" tabRatio="688" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="231">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -758,6 +758,15 @@
   </si>
   <si>
     <t>Set_32b</t>
+  </si>
+  <si>
+    <t>50388930 (Eddie)</t>
+  </si>
+  <si>
+    <t>Set_32c</t>
+  </si>
+  <si>
+    <t>Full simulations with dominance (k = 0)</t>
   </si>
 </sst>
 </file>
@@ -1028,6 +1037,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1046,7 +1056,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1361,13 +1370,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F767BA-E529-4BB9-8A9B-635D3AE84CE5}">
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D42" sqref="D42"/>
+      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2230,13 +2239,13 @@
       </c>
       <c r="J20" s="21"/>
       <c r="K20" s="21"/>
-      <c r="L20" s="45">
+      <c r="L20" s="46">
         <v>45798</v>
       </c>
-      <c r="M20" s="47" t="s">
+      <c r="M20" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="N20" s="45">
+      <c r="N20" s="46">
         <v>45800</v>
       </c>
       <c r="O20" s="23"/>
@@ -2271,9 +2280,9 @@
       </c>
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
-      <c r="L21" s="46"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="46"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="47"/>
       <c r="O21" s="23"/>
     </row>
     <row r="22" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2444,10 +2453,10 @@
       <c r="K25" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L25" s="42">
+      <c r="L25" s="43">
         <v>45843</v>
       </c>
-      <c r="M25" s="44" t="s">
+      <c r="M25" s="45" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2485,8 +2494,8 @@
       <c r="K26" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L26" s="43"/>
-      <c r="M26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="45"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="28" t="s">
@@ -2598,14 +2607,14 @@
       <c r="K29" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L29" s="42">
+      <c r="L29" s="43">
         <v>45854</v>
       </c>
-      <c r="M29" s="44" t="s">
+      <c r="M29" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="N29" s="44"/>
-      <c r="O29" s="44"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="45"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="28" t="s">
@@ -2641,10 +2650,10 @@
       <c r="K30" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L30" s="43"/>
-      <c r="M30" s="44"/>
-      <c r="N30" s="44"/>
-      <c r="O30" s="44"/>
+      <c r="L30" s="44"/>
+      <c r="M30" s="45"/>
+      <c r="N30" s="45"/>
+      <c r="O30" s="45"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="28" t="s">
@@ -2680,10 +2689,10 @@
       <c r="K31" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L31" s="43"/>
-      <c r="M31" s="44"/>
-      <c r="N31" s="44"/>
-      <c r="O31" s="44"/>
+      <c r="L31" s="44"/>
+      <c r="M31" s="45"/>
+      <c r="N31" s="45"/>
+      <c r="O31" s="45"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
@@ -3032,6 +3041,9 @@
       <c r="E40" s="31" t="s">
         <v>219</v>
       </c>
+      <c r="F40" s="2">
+        <v>45881</v>
+      </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="28" t="s">
@@ -3045,6 +3057,20 @@
       </c>
       <c r="D41" s="2">
         <v>45881</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A42" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="C42" s="36">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -3436,13 +3462,13 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="42" t="s">
         <v>222</v>
       </c>
-      <c r="C18" s="48">
+      <c r="C18" s="42">
         <v>100</v>
       </c>
       <c r="D18" s="2">
@@ -3453,24 +3479,24 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="C19" s="48">
+      <c r="C19" s="42">
         <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="42" t="s">
         <v>224</v>
       </c>
-      <c r="C20" s="48">
+      <c r="C20" s="42">
         <v>100</v>
       </c>
     </row>
@@ -3762,11 +3788,11 @@
       <c r="C14" s="29">
         <v>100</v>
       </c>
-      <c r="D14" s="42">
+      <c r="D14" s="43">
         <v>45854</v>
       </c>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44" t="s">
+      <c r="E14" s="45"/>
+      <c r="F14" s="45" t="s">
         <v>162</v>
       </c>
     </row>
@@ -3780,9 +3806,9 @@
       <c r="C15" s="29">
         <v>100</v>
       </c>
-      <c r="D15" s="42"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="28" t="s">
@@ -3794,9 +3820,9 @@
       <c r="C16" s="29">
         <v>100</v>
       </c>
-      <c r="D16" s="42"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">

</xml_diff>

<commit_message>
Set_29 poolseq 1000x params
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E5C27C-8C3D-4EA9-A91E-EF968D06D634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14076512-2399-4966-BE76-BB6D039C2A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="232">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -767,6 +767,9 @@
   </si>
   <si>
     <t>Full simulations with dominance (k = 0)</t>
+  </si>
+  <si>
+    <t>Eddie 50423799</t>
   </si>
 </sst>
 </file>
@@ -1372,7 +1375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F767BA-E529-4BB9-8A9B-635D3AE84CE5}">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3095,8 +3098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B83F06-536D-4FC4-A19B-2685788EFCD2}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3477,6 +3480,9 @@
       <c r="E18" t="s">
         <v>226</v>
       </c>
+      <c r="F18" s="2">
+        <v>45883</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="42" t="s">
@@ -3487,6 +3493,12 @@
       </c>
       <c r="C19" s="42">
         <v>100</v>
+      </c>
+      <c r="D19" s="2">
+        <v>45884</v>
+      </c>
+      <c r="E19" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Set_26 poolseq (500x) and Set_32c params
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14076512-2399-4966-BE76-BB6D039C2A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EE5BE3-C4A4-4E88-887A-D38A03822F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="236">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -770,6 +770,18 @@
   </si>
   <si>
     <t>Eddie 50423799</t>
+  </si>
+  <si>
+    <t>Eddie 50439380</t>
+  </si>
+  <si>
+    <t>Simplified simulations varying the number of neutral sites (read_length = 75, coverage = 00, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Simplified simulations varying the number of neutral sites (read_length = 75, coverage = 100, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Only taskes 1-87 ran, the rest had more than 67500 segregating sites</t>
   </si>
 </sst>
 </file>
@@ -1375,11 +1387,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F767BA-E529-4BB9-8A9B-635D3AE84CE5}">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
+      <selection pane="bottomRight" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3047,6 +3059,21 @@
       <c r="F40" s="2">
         <v>45881</v>
       </c>
+      <c r="G40" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="K40" s="29" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="28" t="s">
@@ -3063,6 +3090,24 @@
       </c>
       <c r="E41" s="31" t="s">
         <v>228</v>
+      </c>
+      <c r="F41" s="2">
+        <v>45885</v>
+      </c>
+      <c r="G41" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="H41" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I41" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="K41" s="29" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
@@ -3096,10 +3141,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B83F06-536D-4FC4-A19B-2685788EFCD2}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3369,79 +3414,63 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="B13" t="s">
-        <v>201</v>
+        <v>233</v>
       </c>
       <c r="C13">
         <v>100</v>
       </c>
-      <c r="D13" s="2">
-        <v>45877</v>
-      </c>
-      <c r="E13" t="s">
-        <v>202</v>
-      </c>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B14" t="s">
+        <v>234</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" t="s">
+        <v>201</v>
+      </c>
+      <c r="C15">
+        <v>100</v>
+      </c>
+      <c r="D15" s="2">
+        <v>45877</v>
+      </c>
+      <c r="E15" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>188</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B16" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="C14">
-        <v>100</v>
-      </c>
-      <c r="D14" s="2">
+      <c r="C16">
+        <v>100</v>
+      </c>
+      <c r="D16" s="2">
         <v>45877</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E16" t="s">
         <v>214</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F16" s="2">
         <v>45879</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="39" t="s">
-        <v>204</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="C15" s="40">
-        <v>100</v>
-      </c>
-      <c r="D15" s="41">
-        <v>45877</v>
-      </c>
-      <c r="E15" t="s">
-        <v>212</v>
-      </c>
-      <c r="F15" s="2">
-        <v>45877</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="39" t="s">
-        <v>204</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="C16" s="40">
-        <v>100</v>
-      </c>
-      <c r="D16" s="41">
-        <v>45877</v>
-      </c>
-      <c r="E16" t="s">
-        <v>213</v>
-      </c>
-      <c r="F16" s="2">
-        <v>45877</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -3449,7 +3478,7 @@
         <v>204</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C17" s="40">
         <v>100</v>
@@ -3458,47 +3487,50 @@
         <v>45877</v>
       </c>
       <c r="E17" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F17" s="2">
         <v>45877</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="42" t="s">
-        <v>217</v>
-      </c>
-      <c r="B18" s="42" t="s">
-        <v>222</v>
-      </c>
-      <c r="C18" s="42">
-        <v>100</v>
-      </c>
-      <c r="D18" s="2">
-        <v>45881</v>
+      <c r="A18" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="C18" s="40">
+        <v>100</v>
+      </c>
+      <c r="D18" s="41">
+        <v>45877</v>
       </c>
       <c r="E18" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="F18" s="2">
-        <v>45883</v>
+        <v>45877</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="42" t="s">
-        <v>217</v>
-      </c>
-      <c r="B19" s="42" t="s">
-        <v>223</v>
-      </c>
-      <c r="C19" s="42">
-        <v>100</v>
-      </c>
-      <c r="D19" s="2">
-        <v>45884</v>
+      <c r="A19" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="C19" s="40">
+        <v>100</v>
+      </c>
+      <c r="D19" s="41">
+        <v>45877</v>
       </c>
       <c r="E19" t="s">
-        <v>231</v>
+        <v>215</v>
+      </c>
+      <c r="F19" s="2">
+        <v>45877</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -3506,10 +3538,56 @@
         <v>217</v>
       </c>
       <c r="B20" s="42" t="s">
+        <v>222</v>
+      </c>
+      <c r="C20" s="42">
+        <v>100</v>
+      </c>
+      <c r="D20" s="2">
+        <v>45881</v>
+      </c>
+      <c r="E20" t="s">
+        <v>226</v>
+      </c>
+      <c r="F20" s="2">
+        <v>45883</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="42" t="s">
+        <v>217</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>223</v>
+      </c>
+      <c r="C21" s="42">
+        <v>100</v>
+      </c>
+      <c r="D21" s="2">
+        <v>45884</v>
+      </c>
+      <c r="E21" t="s">
+        <v>231</v>
+      </c>
+      <c r="F21" s="2">
+        <v>45884</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="42" t="s">
+        <v>217</v>
+      </c>
+      <c r="B22" s="42" t="s">
         <v>224</v>
       </c>
-      <c r="C20" s="42">
-        <v>100</v>
+      <c r="C22" s="42">
+        <v>100</v>
+      </c>
+      <c r="D22" s="2">
+        <v>45884</v>
+      </c>
+      <c r="E22" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set_26 poolseq 100x params
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22288E1D-1184-4B84-9BC5-76E108EA5C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FCC34B-9D1E-4392-9746-34BD30AC76FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -790,10 +790,10 @@
     <t>50447801 (Eddie)</t>
   </si>
   <si>
-    <t>following tasks were timed out: 52, 65, 89, 97, 98, 99</t>
-  </si>
-  <si>
-    <t>Only tasks 1-47 ran the rest were timed out; rerun as</t>
+    <t>following tasks were timed out: 52, 65, 89, 97, 98, 99; rerun as 50449683, 50449684, 50449687, 50449688, 50449690, 50449692, respectively</t>
+  </si>
+  <si>
+    <t>Only tasks 1-47 ran the rest were timed out; rerun as 50449698 (Eddie)</t>
   </si>
 </sst>
 </file>
@@ -1400,7 +1400,7 @@
   <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G43" sqref="G43"/>
@@ -3164,8 +3164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B83F06-536D-4FC4-A19B-2685788EFCD2}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Set_32 new va calculation params
Also some backup Latex code for the manuscript
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C65742F-15BA-4DD0-9971-89D87E4F3B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2432EF8D-583F-487D-956D-2ED4254D96B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="243">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -800,6 +800,9 @@
   </si>
   <si>
     <t>Tasks 52 and 65 were rerun as 50454515 and 50454516</t>
+  </si>
+  <si>
+    <t>50455814 (Eddie)</t>
   </si>
 </sst>
 </file>
@@ -1409,7 +1412,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="G30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M40" sqref="M40:M42"/>
+      <selection pane="bottomRight" activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3095,7 +3098,9 @@
       <c r="L40" s="43">
         <v>45887</v>
       </c>
-      <c r="M40" s="45"/>
+      <c r="M40" s="45" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="28" t="s">

</xml_diff>

<commit_message>
Extract data for plotting UL vs positions
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2432EF8D-583F-487D-956D-2ED4254D96B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E61D2A-C108-4AFA-ADCE-8668EF245FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" activeTab="2" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="246">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -803,6 +803,15 @@
   </si>
   <si>
     <t>50455814 (Eddie)</t>
+  </si>
+  <si>
+    <t>Set_32</t>
+  </si>
+  <si>
+    <t>Full simulations with dominance (k = 0, k = 0.5, k = 0.75)</t>
+  </si>
+  <si>
+    <t>50461156 (Eddie)</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1021,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1091,6 +1100,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1408,11 +1420,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F767BA-E529-4BB9-8A9B-635D3AE84CE5}">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G30" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M43" sqref="M43"/>
+      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3101,6 +3113,9 @@
       <c r="M40" s="45" t="s">
         <v>242</v>
       </c>
+      <c r="N40" s="49">
+        <v>45888</v>
+      </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="28" t="s">
@@ -3138,6 +3153,7 @@
       </c>
       <c r="L41" s="44"/>
       <c r="M41" s="45"/>
+      <c r="N41" s="45"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="28" t="s">
@@ -3172,11 +3188,13 @@
       </c>
       <c r="L42" s="44"/>
       <c r="M42" s="45"/>
+      <c r="N42" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="L40:L42"/>
     <mergeCell ref="M40:M42"/>
+    <mergeCell ref="N40:N42"/>
     <mergeCell ref="L29:L31"/>
     <mergeCell ref="M29:M31"/>
     <mergeCell ref="N29:N31"/>
@@ -3673,10 +3691,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E757BB-1C2C-4D1E-BA64-CFB54311D593}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4085,6 +4103,23 @@
       </c>
       <c r="F22" t="s">
         <v>198</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B23" t="s">
+        <v>244</v>
+      </c>
+      <c r="C23" s="36">
+        <v>285</v>
+      </c>
+      <c r="D23" s="2">
+        <v>45888</v>
+      </c>
+      <c r="F23" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding coverage to analysis
Modified extratc_slim_data() and analyse_sim() to accommodate coverage1 and coverage2
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEA38A3-E6C9-4226-820C-BCDFC4D0C847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705270B4-D02C-44FE-AC53-B33BB28C2630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="688" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -816,7 +816,7 @@
     <t>Standard set without burnin analysed with simulations pf poolseq (read_length = 1e+6, coverage = 100, V_logmean = 0)</t>
   </si>
   <si>
-    <t>Eddie 50472227</t>
+    <t>Eddie 50472494</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
poolseq analyses with Q
params for coverage = 500
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705270B4-D02C-44FE-AC53-B33BB28C2630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D7BE2C-7E38-4CDC-8A25-576694506F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="688" activeTab="1" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="688" activeTab="2" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
     <sheet name="Pool_seq_analyses" sheetId="4" r:id="rId2"/>
-    <sheet name="Rcalculate true V_A &amp; V_a_left" sheetId="2" r:id="rId3"/>
-    <sheet name="Recalculate BC_V_A" sheetId="3" r:id="rId4"/>
+    <sheet name="Pool_seq_analysis_with_Q" sheetId="5" r:id="rId3"/>
+    <sheet name="Rcalculate true V_A &amp; V_a_left" sheetId="2" r:id="rId4"/>
+    <sheet name="Recalculate BC_V_A" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,12 +33,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="252">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -817,6 +821,18 @@
   </si>
   <si>
     <t>Eddie 50472494</t>
+  </si>
+  <si>
+    <t>Standard set without burnin analysed with simulations pf poolseq (read_length = 800, coverage = 100, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Eddie 50481523</t>
+  </si>
+  <si>
+    <t>Standard set without burnin analysed with simulations pf poolseq (read_length = 800, coverage = 500, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Standard set without burnin analysed with simulations pf poolseq (read_length = 800, coverage = 1000, V_logmean = 0)</t>
   </si>
 </sst>
 </file>
@@ -1088,16 +1104,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1108,6 +1115,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2292,13 +2308,13 @@
       </c>
       <c r="J20" s="21"/>
       <c r="K20" s="21"/>
-      <c r="L20" s="47">
+      <c r="L20" s="44">
         <v>45798</v>
       </c>
-      <c r="M20" s="49" t="s">
+      <c r="M20" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="N20" s="47">
+      <c r="N20" s="44">
         <v>45800</v>
       </c>
       <c r="O20" s="23"/>
@@ -2333,9 +2349,9 @@
       </c>
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="48"/>
+      <c r="L21" s="45"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="45"/>
       <c r="O21" s="23"/>
     </row>
     <row r="22" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2506,10 +2522,10 @@
       <c r="K25" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L25" s="43">
+      <c r="L25" s="47">
         <v>45843</v>
       </c>
-      <c r="M25" s="45" t="s">
+      <c r="M25" s="43" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2547,8 +2563,8 @@
       <c r="K26" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L26" s="44"/>
-      <c r="M26" s="45"/>
+      <c r="L26" s="48"/>
+      <c r="M26" s="43"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="28" t="s">
@@ -2660,14 +2676,14 @@
       <c r="K29" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L29" s="43">
+      <c r="L29" s="47">
         <v>45854</v>
       </c>
-      <c r="M29" s="45" t="s">
+      <c r="M29" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="N29" s="45"/>
-      <c r="O29" s="45"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="43"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="28" t="s">
@@ -2703,10 +2719,10 @@
       <c r="K30" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L30" s="44"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="45"/>
-      <c r="O30" s="45"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="43"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="43"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="28" t="s">
@@ -2742,10 +2758,10 @@
       <c r="K31" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L31" s="44"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="45"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="43"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
@@ -3112,13 +3128,13 @@
       <c r="K40" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L40" s="43">
+      <c r="L40" s="47">
         <v>45887</v>
       </c>
-      <c r="M40" s="45" t="s">
+      <c r="M40" s="43" t="s">
         <v>242</v>
       </c>
-      <c r="N40" s="46">
+      <c r="N40" s="49">
         <v>45888</v>
       </c>
     </row>
@@ -3156,9 +3172,9 @@
       <c r="K41" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L41" s="44"/>
-      <c r="M41" s="45"/>
-      <c r="N41" s="45"/>
+      <c r="L41" s="48"/>
+      <c r="M41" s="43"/>
+      <c r="N41" s="43"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="28" t="s">
@@ -3191,24 +3207,24 @@
       <c r="K42" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L42" s="44"/>
-      <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
+      <c r="L42" s="48"/>
+      <c r="M42" s="43"/>
+      <c r="N42" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="L40:L42"/>
+    <mergeCell ref="M40:M42"/>
+    <mergeCell ref="N40:N42"/>
+    <mergeCell ref="L29:L31"/>
+    <mergeCell ref="M29:M31"/>
+    <mergeCell ref="N29:N31"/>
     <mergeCell ref="O29:O31"/>
     <mergeCell ref="N20:N21"/>
     <mergeCell ref="L20:L21"/>
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="L25:L26"/>
     <mergeCell ref="M25:M26"/>
-    <mergeCell ref="L40:L42"/>
-    <mergeCell ref="M40:M42"/>
-    <mergeCell ref="N40:N42"/>
-    <mergeCell ref="L29:L31"/>
-    <mergeCell ref="M29:M31"/>
-    <mergeCell ref="N29:N31"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3220,8 +3236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B83F06-536D-4FC4-A19B-2685788EFCD2}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3712,6 +3728,99 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60697B5-448A-4649-904A-61CE6DBEF6DE}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45890</v>
+      </c>
+      <c r="E2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45890</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" t="s">
+        <v>250</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45890</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45890</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E757BB-1C2C-4D1E-BA64-CFB54311D593}">
   <dimension ref="A1:G23"/>
   <sheetViews>
@@ -3994,11 +4103,11 @@
       <c r="C14" s="29">
         <v>100</v>
       </c>
-      <c r="D14" s="43">
+      <c r="D14" s="47">
         <v>45854</v>
       </c>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45" t="s">
+      <c r="E14" s="43"/>
+      <c r="F14" s="43" t="s">
         <v>162</v>
       </c>
     </row>
@@ -4012,9 +4121,9 @@
       <c r="C15" s="29">
         <v>100</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="28" t="s">
@@ -4026,9 +4135,9 @@
       <c r="C16" s="29">
         <v>100</v>
       </c>
-      <c r="D16" s="43"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
@@ -4155,7 +4264,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8D10C7-D493-4278-B869-F549E3A19DCB}">
   <dimension ref="A1:F2"/>
   <sheetViews>

</xml_diff>

<commit_message>
poolseq with Q analysis
1000x params
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D7BE2C-7E38-4CDC-8A25-576694506F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAC17B6-2229-472D-85BC-3AF0E1122E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="688" activeTab="2" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="253">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -833,6 +833,9 @@
   </si>
   <si>
     <t>Standard set without burnin analysed with simulations pf poolseq (read_length = 800, coverage = 1000, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Eddie 50481610</t>
   </si>
 </sst>
 </file>
@@ -3732,7 +3735,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3799,6 +3802,9 @@
       </c>
       <c r="D3" s="2">
         <v>45890</v>
+      </c>
+      <c r="E3" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
poolseq with Q analyses
params for overdispered analyses
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAC17B6-2229-472D-85BC-3AF0E1122E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21AF7B51-7F4E-46A8-AF7D-E57B19F44DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="688" activeTab="2" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" tabRatio="688" activeTab="2" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="255">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -836,6 +836,12 @@
   </si>
   <si>
     <t>Eddie 50481610</t>
+  </si>
+  <si>
+    <t>Eddie 50481663</t>
+  </si>
+  <si>
+    <t>Standard set without burnin analysed with simulations pf poolseq (read_length = 800, coverage = 1000, V_logmean = log(2))</t>
   </si>
 </sst>
 </file>
@@ -3732,10 +3738,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60697B5-448A-4649-904A-61CE6DBEF6DE}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3806,6 +3812,9 @@
       <c r="E3" t="s">
         <v>252</v>
       </c>
+      <c r="F3" s="2">
+        <v>45890</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -3818,6 +3827,26 @@
         <v>100</v>
       </c>
       <c r="D4" s="2">
+        <v>45890</v>
+      </c>
+      <c r="E4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45890</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5" s="2">
         <v>45890</v>
       </c>
     </row>

</xml_diff>

<commit_message>
seeds in simulations cripts
also params for poolseq with Q full (500x)
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66442E3-2875-463E-9E98-210AA6EACC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7FAE27-13F3-47DE-B72C-5FA718188F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" tabRatio="688" activeTab="2" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="28635" yWindow="-165" windowWidth="29130" windowHeight="17610" tabRatio="688" activeTab="2" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="259">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -848,6 +848,12 @@
   </si>
   <si>
     <t>Standard set with burnin analysed with simulations pf poolseq (read_length = 37, coverage = 100, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Eddie 50482115</t>
+  </si>
+  <si>
+    <t>Standard set with burnin analysed with simulations pf poolseq (read_length = 37, coverage = 500, V_logmean = 0)</t>
   </si>
 </sst>
 </file>
@@ -3744,10 +3750,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60697B5-448A-4649-904A-61CE6DBEF6DE}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F5" sqref="F5:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3858,6 +3864,9 @@
       <c r="E5" t="s">
         <v>255</v>
       </c>
+      <c r="F5" s="2">
+        <v>45890</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -3871,6 +3880,26 @@
       </c>
       <c r="D6" s="2">
         <v>45890</v>
+      </c>
+      <c r="E6" t="s">
+        <v>257</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45890</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7" s="2">
+        <v>45891</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Poolseq with Q full sims params
coverage = 1000x, V_logmean = log(1)
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18AD966-D4B9-4756-B9C9-31C823F8218B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3846E3B-2AD1-4405-9118-438A27E378BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" tabRatio="688" activeTab="2" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="263">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -860,6 +860,12 @@
   </si>
   <si>
     <t>Standard set with burnin analysed with simulations pf poolseq (read_length = 37, coverage = 1000, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Eddie 50490318</t>
+  </si>
+  <si>
+    <t>Standard set with burnin analysed with simulations pf poolseq (read_length = 37, coverage = 1000, V_logmean = log(2))</t>
   </si>
 </sst>
 </file>
@@ -3756,10 +3762,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60697B5-448A-4649-904A-61CE6DBEF6DE}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3910,6 +3916,9 @@
       <c r="E7" t="s">
         <v>259</v>
       </c>
+      <c r="F7" s="2">
+        <v>45892</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -3922,6 +3931,23 @@
         <v>100</v>
       </c>
       <c r="D8" s="2">
+        <v>45892</v>
+      </c>
+      <c r="E8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9" s="2">
         <v>45892</v>
       </c>
     </row>

</xml_diff>

<commit_message>
poolseq analyses without Q
Simplified sims (100x)
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3846E3B-2AD1-4405-9118-438A27E378BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9900EC53-7936-40AF-B853-AD1F0E6D38A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" tabRatio="688" activeTab="2" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" activeTab="2" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sims and main analysis" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="265">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -823,49 +823,55 @@
     <t>Eddie 50472494</t>
   </si>
   <si>
-    <t>Standard set without burnin analysed with simulations pf poolseq (read_length = 800, coverage = 100, V_logmean = 0)</t>
-  </si>
-  <si>
     <t>Eddie 50481523</t>
   </si>
   <si>
-    <t>Standard set without burnin analysed with simulations pf poolseq (read_length = 800, coverage = 500, V_logmean = 0)</t>
-  </si>
-  <si>
-    <t>Standard set without burnin analysed with simulations pf poolseq (read_length = 800, coverage = 1000, V_logmean = 0)</t>
-  </si>
-  <si>
     <t>Eddie 50481610</t>
   </si>
   <si>
     <t>Eddie 50481663</t>
   </si>
   <si>
-    <t>Standard set without burnin analysed with simulations pf poolseq (read_length = 800, coverage = 1000, V_logmean = log(2))</t>
-  </si>
-  <si>
     <t>Eddie 50481894</t>
   </si>
   <si>
-    <t>Standard set with burnin analysed with simulations pf poolseq (read_length = 37, coverage = 100, V_logmean = 0)</t>
-  </si>
-  <si>
     <t>Eddie 50482115</t>
   </si>
   <si>
-    <t>Standard set with burnin analysed with simulations pf poolseq (read_length = 37, coverage = 500, V_logmean = 0)</t>
-  </si>
-  <si>
     <t>Eddie 50484406</t>
   </si>
   <si>
-    <t>Standard set with burnin analysed with simulations pf poolseq (read_length = 37, coverage = 1000, V_logmean = 0)</t>
-  </si>
-  <si>
     <t>Eddie 50490318</t>
   </si>
   <si>
-    <t>Standard set with burnin analysed with simulations pf poolseq (read_length = 37, coverage = 1000, V_logmean = log(2))</t>
+    <t>Eddie 50491953</t>
+  </si>
+  <si>
+    <t>Standard set without burnin analysed with simulations of poolseq (incorporateQ = FALSE, read_length = 800, coverage = 100, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Standard set with burnin analysed with simulations of poolseq (read_length = 37, coverage = 1000, V_logmean = log(2))</t>
+  </si>
+  <si>
+    <t>Standard set with burnin analysed with simulations of poolseq (read_length = 37, coverage = 1000, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Standard set without burnin analysed with simulations of poolseq (read_length = 800, coverage = 100, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Standard set without burnin analysed with simulations of poolseq (read_length = 800, coverage = 500, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Standard set without burnin analysed with simulations of poolseq (read_length = 800, coverage = 1000, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Standard set without burnin analysed with simulations of poolseq (read_length = 800, coverage = 1000, V_logmean = log(2))</t>
+  </si>
+  <si>
+    <t>Standard set with burnin analysed with simulations of poolseq (read_length = 37, coverage = 100, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Standard set with burnin analysed with simulations of poolseq (read_length = 37, coverage = 500, V_logmean = 0)</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1143,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1148,15 +1163,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2341,13 +2347,13 @@
       </c>
       <c r="J20" s="21"/>
       <c r="K20" s="21"/>
-      <c r="L20" s="44">
+      <c r="L20" s="47">
         <v>45798</v>
       </c>
-      <c r="M20" s="46" t="s">
+      <c r="M20" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="N20" s="44">
+      <c r="N20" s="47">
         <v>45800</v>
       </c>
       <c r="O20" s="23"/>
@@ -2382,9 +2388,9 @@
       </c>
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="46"/>
-      <c r="N21" s="45"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="48"/>
       <c r="O21" s="23"/>
     </row>
     <row r="22" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2555,10 +2561,10 @@
       <c r="K25" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L25" s="47">
+      <c r="L25" s="43">
         <v>45843</v>
       </c>
-      <c r="M25" s="43" t="s">
+      <c r="M25" s="45" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2596,8 +2602,8 @@
       <c r="K26" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L26" s="48"/>
-      <c r="M26" s="43"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="45"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="28" t="s">
@@ -2709,14 +2715,14 @@
       <c r="K29" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L29" s="47">
+      <c r="L29" s="43">
         <v>45854</v>
       </c>
-      <c r="M29" s="43" t="s">
+      <c r="M29" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="N29" s="43"/>
-      <c r="O29" s="43"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="45"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="28" t="s">
@@ -2752,10 +2758,10 @@
       <c r="K30" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L30" s="48"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="43"/>
-      <c r="O30" s="43"/>
+      <c r="L30" s="44"/>
+      <c r="M30" s="45"/>
+      <c r="N30" s="45"/>
+      <c r="O30" s="45"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="28" t="s">
@@ -2791,10 +2797,10 @@
       <c r="K31" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L31" s="48"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="43"/>
-      <c r="O31" s="43"/>
+      <c r="L31" s="44"/>
+      <c r="M31" s="45"/>
+      <c r="N31" s="45"/>
+      <c r="O31" s="45"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
@@ -3161,13 +3167,13 @@
       <c r="K40" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L40" s="47">
+      <c r="L40" s="43">
         <v>45887</v>
       </c>
-      <c r="M40" s="43" t="s">
+      <c r="M40" s="45" t="s">
         <v>242</v>
       </c>
-      <c r="N40" s="49">
+      <c r="N40" s="46">
         <v>45888</v>
       </c>
     </row>
@@ -3205,9 +3211,9 @@
       <c r="K41" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L41" s="48"/>
-      <c r="M41" s="43"/>
-      <c r="N41" s="43"/>
+      <c r="L41" s="44"/>
+      <c r="M41" s="45"/>
+      <c r="N41" s="45"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="28" t="s">
@@ -3240,24 +3246,24 @@
       <c r="K42" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L42" s="48"/>
-      <c r="M42" s="43"/>
-      <c r="N42" s="43"/>
+      <c r="L42" s="44"/>
+      <c r="M42" s="45"/>
+      <c r="N42" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="O29:O31"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="M25:M26"/>
     <mergeCell ref="L40:L42"/>
     <mergeCell ref="M40:M42"/>
     <mergeCell ref="N40:N42"/>
     <mergeCell ref="L29:L31"/>
     <mergeCell ref="M29:M31"/>
     <mergeCell ref="N29:N31"/>
-    <mergeCell ref="O29:O31"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="M25:M26"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3762,10 +3768,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60697B5-448A-4649-904A-61CE6DBEF6DE}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3805,7 +3811,7 @@
         <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -3814,7 +3820,7 @@
         <v>45890</v>
       </c>
       <c r="E2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F2" s="2">
         <v>45890</v>
@@ -3825,7 +3831,7 @@
         <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -3834,7 +3840,7 @@
         <v>45890</v>
       </c>
       <c r="E3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F3" s="2">
         <v>45890</v>
@@ -3845,7 +3851,7 @@
         <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -3854,7 +3860,7 @@
         <v>45890</v>
       </c>
       <c r="E4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F4" s="2">
         <v>45890</v>
@@ -3865,7 +3871,7 @@
         <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -3874,7 +3880,7 @@
         <v>45890</v>
       </c>
       <c r="E5" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F5" s="2">
         <v>45890</v>
@@ -3885,7 +3891,7 @@
         <v>122</v>
       </c>
       <c r="B6" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -3894,7 +3900,7 @@
         <v>45890</v>
       </c>
       <c r="E6" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="F6" s="2">
         <v>45890</v>
@@ -3905,7 +3911,7 @@
         <v>122</v>
       </c>
       <c r="B7" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C7">
         <v>100</v>
@@ -3914,7 +3920,7 @@
         <v>45891</v>
       </c>
       <c r="E7" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="F7" s="2">
         <v>45892</v>
@@ -3925,7 +3931,7 @@
         <v>122</v>
       </c>
       <c r="B8" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C8">
         <v>100</v>
@@ -3934,7 +3940,10 @@
         <v>45892</v>
       </c>
       <c r="E8" t="s">
-        <v>261</v>
+        <v>254</v>
+      </c>
+      <c r="F8" s="2">
+        <v>45892</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -3942,13 +3951,27 @@
         <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C9">
         <v>100</v>
       </c>
       <c r="D9" s="2">
         <v>45892</v>
+      </c>
+      <c r="E9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -4239,11 +4262,11 @@
       <c r="C14" s="29">
         <v>100</v>
       </c>
-      <c r="D14" s="47">
+      <c r="D14" s="43">
         <v>45854</v>
       </c>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43" t="s">
+      <c r="E14" s="45"/>
+      <c r="F14" s="45" t="s">
         <v>162</v>
       </c>
     </row>
@@ -4257,9 +4280,9 @@
       <c r="C15" s="29">
         <v>100</v>
       </c>
-      <c r="D15" s="47"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="28" t="s">
@@ -4271,9 +4294,9 @@
       <c r="C16" s="29">
         <v>100</v>
       </c>
-      <c r="D16" s="47"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">

</xml_diff>

<commit_message>
poolseq analyses noQ simmplified sims
500x
</commit_message>
<xml_diff>
--- a/3_logs/Vw_sim_logs.xlsx
+++ b/3_logs/Vw_sim_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msamant\Documents\GitHub\Va_simulations\3_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9900EC53-7936-40AF-B853-AD1F0E6D38A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7657B92-CEC7-4C4B-AFB7-672DB626D504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="688" activeTab="2" xr2:uid="{54A405BA-125B-4F10-BE8B-8201627BA33E}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="267">
   <si>
     <t>Set_ID_prefix</t>
   </si>
@@ -872,6 +872,12 @@
   </si>
   <si>
     <t>Standard set with burnin analysed with simulations of poolseq (read_length = 37, coverage = 500, V_logmean = 0)</t>
+  </si>
+  <si>
+    <t>Eddie 50494477</t>
+  </si>
+  <si>
+    <t>Standard set without burnin analysed with simulations of poolseq (incorporateQ = FALSE, read_length = 800, coverage = 500, V_logmean = 0)</t>
   </si>
 </sst>
 </file>
@@ -3768,10 +3774,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60697B5-448A-4649-904A-61CE6DBEF6DE}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3962,6 +3968,9 @@
       <c r="E9" t="s">
         <v>255</v>
       </c>
+      <c r="F9" s="2">
+        <v>45893</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -3972,6 +3981,29 @@
       </c>
       <c r="C10">
         <v>100</v>
+      </c>
+      <c r="D10" s="2">
+        <v>45893</v>
+      </c>
+      <c r="E10" t="s">
+        <v>265</v>
+      </c>
+      <c r="F10" s="2">
+        <v>45893</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" t="s">
+        <v>266</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11" s="2">
+        <v>45893</v>
       </c>
     </row>
   </sheetData>

</xml_diff>